<commit_message>
add more days schedules for processed data
</commit_message>
<xml_diff>
--- a/data/horarios-de-nivelacion-procesados.xlsx
+++ b/data/horarios-de-nivelacion-procesados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dev\Documents\GitHub\fcc-pregrado-horarios-y-matriculas-xlsx-to-json\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7259707-9292-43B3-95CB-D443EBE7F1B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA733A2F-AC32-41B8-B758-5B609CAC41FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{99FAE42D-B215-4180-9DA5-7D453DC9DB15}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{99FAE42D-B215-4180-9DA5-7D453DC9DB15}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="163">
   <si>
     <t>ciclo</t>
   </si>
@@ -411,13 +411,127 @@
   </si>
   <si>
     <t>GERARDO MANUEL</t>
+  </si>
+  <si>
+    <t>113443</t>
+  </si>
+  <si>
+    <t>113450</t>
+  </si>
+  <si>
+    <t>111443</t>
+  </si>
+  <si>
+    <t>111450</t>
+  </si>
+  <si>
+    <t>112443</t>
+  </si>
+  <si>
+    <t>112450</t>
+  </si>
+  <si>
+    <t>404</t>
+  </si>
+  <si>
+    <t>FUNDAMENTOS DE FINANZAS</t>
+  </si>
+  <si>
+    <t>08628745</t>
+  </si>
+  <si>
+    <t>GARCÍA</t>
+  </si>
+  <si>
+    <t>VILLEGAS</t>
+  </si>
+  <si>
+    <t>EMILIO GABRIEL</t>
+  </si>
+  <si>
+    <t>LUNES</t>
+  </si>
+  <si>
+    <t>114402</t>
+  </si>
+  <si>
+    <t>PFP</t>
+  </si>
+  <si>
+    <t>111647</t>
+  </si>
+  <si>
+    <t>DERECHO TRIBUTARIO II</t>
+  </si>
+  <si>
+    <t>23929930</t>
+  </si>
+  <si>
+    <t>ZUÑIGA</t>
+  </si>
+  <si>
+    <t>HERMOSA</t>
+  </si>
+  <si>
+    <t>DANITZA</t>
+  </si>
+  <si>
+    <t>111782</t>
+  </si>
+  <si>
+    <t>112741</t>
+  </si>
+  <si>
+    <t>113741</t>
+  </si>
+  <si>
+    <t>INFORMACION FINANCIERA</t>
+  </si>
+  <si>
+    <t>INFORMACIÓN FINANCIERA</t>
+  </si>
+  <si>
+    <t>308</t>
+  </si>
+  <si>
+    <t>25406615</t>
+  </si>
+  <si>
+    <t>LOLI</t>
+  </si>
+  <si>
+    <t>BONILLA</t>
+  </si>
+  <si>
+    <t>CESAR ENRIQUE</t>
+  </si>
+  <si>
+    <t>112046</t>
+  </si>
+  <si>
+    <t>TRIBUTACION INTERNACIONAL II</t>
+  </si>
+  <si>
+    <t>23937445</t>
+  </si>
+  <si>
+    <t>AGUIRRE</t>
+  </si>
+  <si>
+    <t>ARREDONDO</t>
+  </si>
+  <si>
+    <t>NANCY</t>
+  </si>
+  <si>
+    <t>19:15</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -425,8 +539,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -481,6 +601,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -494,7 +632,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -513,6 +651,12 @@
     <xf numFmtId="49" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -682,8 +826,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DC0E0ADC-44B0-4CEF-BCCC-97D20B41F157}" name="Table1" displayName="Table1" ref="A1:Q34" totalsRowShown="0" dataDxfId="17">
-  <autoFilter ref="A1:Q34" xr:uid="{DC0E0ADC-44B0-4CEF-BCCC-97D20B41F157}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DC0E0ADC-44B0-4CEF-BCCC-97D20B41F157}" name="Table1" displayName="Table1" ref="A1:Q47" totalsRowShown="0" dataDxfId="17">
+  <autoFilter ref="A1:Q47" xr:uid="{DC0E0ADC-44B0-4CEF-BCCC-97D20B41F157}"/>
   <tableColumns count="17">
     <tableColumn id="1" xr3:uid="{0A177087-4C15-4674-A4A9-7D9BD880913A}" name="ciclo" dataDxfId="16"/>
     <tableColumn id="2" xr3:uid="{8DF6EEB5-31DE-43FB-8CC5-CF192B52A0D0}" name="escuela" dataDxfId="15"/>
@@ -1024,10 +1168,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1746F96C-94FA-48F7-B6FA-3EEFCDB601C7}">
-  <dimension ref="A1:Q34"/>
+  <dimension ref="A1:Q47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2774,7 +2918,7 @@
         <v>57</v>
       </c>
       <c r="N33" s="14" t="b">
-        <f t="shared" ref="N33:N34" si="11">NOT(ISBLANK(O33))</f>
+        <f t="shared" ref="N33:N41" si="11">NOT(ISBLANK(O33))</f>
         <v>1</v>
       </c>
       <c r="O33" s="14" t="s">
@@ -2835,7 +2979,680 @@
       <c r="P34" s="17"/>
       <c r="Q34" s="17"/>
     </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A35" s="18">
+        <v>4</v>
+      </c>
+      <c r="B35" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C35" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="D35" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="E35" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="F35" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="G35" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="H35" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="I35" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="J35" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="K35" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="L35" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="M35" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="N35" s="18" t="b">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="O35" s="18"/>
+      <c r="P35" s="19"/>
+      <c r="Q35" s="19"/>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A36" s="18">
+        <v>4</v>
+      </c>
+      <c r="B36" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C36" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="D36" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="E36" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="F36" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="G36" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="H36" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="I36" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="J36" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="K36" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="L36" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="M36" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="N36" s="18" t="b">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="O36" s="18"/>
+      <c r="P36" s="19"/>
+      <c r="Q36" s="19"/>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A37" s="18">
+        <v>4</v>
+      </c>
+      <c r="B37" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C37" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="D37" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="E37" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="F37" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="G37" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="H37" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="I37" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="J37" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="K37" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="L37" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="M37" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="N37" s="18" t="b">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="O37" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="P37" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q37" s="19" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A38" s="18">
+        <v>4</v>
+      </c>
+      <c r="B38" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="C38" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="D38" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="E38" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="F38" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="G38" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="H38" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="I38" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="J38" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="K38" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="L38" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="M38" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="N38" s="18" t="b">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="O38" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="P38" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q38" s="19" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A39" s="18">
+        <v>4</v>
+      </c>
+      <c r="B39" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="C39" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="D39" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="E39" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="F39" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="G39" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="H39" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="I39" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="J39" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="K39" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="L39" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="M39" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="N39" s="18" t="b">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="O39" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="P39" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q39" s="19" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A40" s="18">
+        <v>4</v>
+      </c>
+      <c r="B40" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C40" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="D40" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="E40" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="F40" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="G40" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="H40" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="I40" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="J40" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="K40" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="L40" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="M40" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="N40" s="18" t="b">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="O40" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="P40" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q40" s="19" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A41" s="18">
+        <v>4</v>
+      </c>
+      <c r="B41" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C41" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="D41" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="E41" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="F41" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="G41" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="H41" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="I41" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="J41" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="K41" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="L41" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="M41" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="N41" s="18" t="b">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="O41" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="P41" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q41" s="19" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A42" s="20">
+        <v>4</v>
+      </c>
+      <c r="B42" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="C42" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="D42" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="E42" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="F42" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="G42" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="H42" s="20" t="s">
+        <v>134</v>
+      </c>
+      <c r="I42" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="J42" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="K42" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="L42" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="M42" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="N42" s="20" t="b">
+        <f t="shared" ref="N42:N43" si="12">NOT(ISBLANK(O42))</f>
+        <v>1</v>
+      </c>
+      <c r="O42" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="P42" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q42" s="21" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A43" s="22">
+        <v>6</v>
+      </c>
+      <c r="B43" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C43" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="D43" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="E43" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="F43" s="23" t="s">
+        <v>131</v>
+      </c>
+      <c r="G43" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="H43" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="I43" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="J43" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="K43" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="L43" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="M43" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="N43" s="22" t="b">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="O43" s="22"/>
+      <c r="P43" s="23"/>
+      <c r="Q43" s="23"/>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A44" s="8">
+        <v>7</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="E44" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="F44" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="G44" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="H44" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="I44" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="J44" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="K44" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="L44" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="M44" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="N44" s="8" t="b">
+        <f t="shared" ref="N44:N47" si="13">NOT(ISBLANK(O44))</f>
+        <v>0</v>
+      </c>
+      <c r="O44" s="8"/>
+      <c r="P44" s="9"/>
+      <c r="Q44" s="9"/>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A45" s="8">
+        <v>7</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="E45" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="F45" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="G45" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="H45" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="I45" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="J45" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="K45" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="L45" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="M45" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="N45" s="8" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="O45" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="P45" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q45" s="9" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A46" s="8">
+        <v>7</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="E46" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="F46" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="G46" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="H46" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="I46" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="J46" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="K46" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="L46" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="M46" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="N46" s="8" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="O46" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="P46" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q46" s="9" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A47" s="2">
+        <v>10</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="I47" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="J47" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="K47" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="L47" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="M47" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="N47" s="2" t="b">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="O47" s="2"/>
+      <c r="P47" s="3"/>
+      <c r="Q47" s="3"/>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>